<commit_message>
changes on IORM objective
</commit_message>
<xml_diff>
--- a/eco_2015/DBRM IORM Testcase Matrix.xlsx
+++ b/eco_2015/DBRM IORM Testcase Matrix.xlsx
@@ -902,7 +902,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="234">
   <si>
     <t>cdb1</t>
   </si>
@@ -2056,6 +2056,9 @@
   <si>
     <t>(DEFAULT)</t>
   </si>
+  <si>
+    <t>&gt; IORM objective to AUTO or BALANCED</t>
+  </si>
 </sst>
 </file>
 
@@ -5017,7 +5020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AT653"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5144,7 +5149,7 @@
         <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="V3" t="s">
         <v>14</v>
@@ -5469,7 +5474,7 @@
         <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="V11" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Revert "changes on IORM objective"
This reverts commit 64773ed6ba8c1f39490512c92e0e1cd42a340754.
</commit_message>
<xml_diff>
--- a/eco_2015/DBRM IORM Testcase Matrix.xlsx
+++ b/eco_2015/DBRM IORM Testcase Matrix.xlsx
@@ -902,7 +902,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="233">
   <si>
     <t>cdb1</t>
   </si>
@@ -2056,9 +2056,6 @@
   <si>
     <t>(DEFAULT)</t>
   </si>
-  <si>
-    <t>&gt; IORM objective to AUTO or BALANCED</t>
-  </si>
 </sst>
 </file>
 
@@ -5020,9 +5017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AT653"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5149,7 +5144,7 @@
         <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
       <c r="V3" t="s">
         <v>14</v>
@@ -5474,7 +5469,7 @@
         <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
       <c r="V11" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
change on IORM objective
</commit_message>
<xml_diff>
--- a/eco_2015/DBRM IORM Testcase Matrix.xlsx
+++ b/eco_2015/DBRM IORM Testcase Matrix.xlsx
@@ -902,7 +902,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="234">
   <si>
     <t>cdb1</t>
   </si>
@@ -2056,6 +2056,9 @@
   <si>
     <t>(DEFAULT)</t>
   </si>
+  <si>
+    <t>&gt; IORM objective to AUTO or BALANCED</t>
+  </si>
 </sst>
 </file>
 
@@ -5017,7 +5020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AT653"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5144,7 +5149,7 @@
         <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="V3" t="s">
         <v>14</v>
@@ -5469,7 +5474,7 @@
         <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="V11" t="s">
         <v>35</v>

</xml_diff>